<commit_message>
NUM STRING y SLIDE andando
</commit_message>
<xml_diff>
--- a/archivo3.xlsx
+++ b/archivo3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fidel\Desktop\pue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D532FAD3-38A6-449D-AF01-8376A3F52425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985E7396-5BA5-4F31-8C93-51F39C1E3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,8 @@
   </sheets>
   <definedNames>
     <definedName name="PUE.NUM.edad2">Sheet1!$D$4</definedName>
+    <definedName name="PUE.SLIDE.0.1.0.1.porcentaje1">Sheet1!$B$11</definedName>
+    <definedName name="PUE.STRING.cadena1">Sheet1!$G$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -452,7 +454,7 @@
   <dimension ref="B2:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Agrega soporte para rangos de NUM, STRING y SWITCH
</commit_message>
<xml_diff>
--- a/archivo3.xlsx
+++ b/archivo3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fidel\Desktop\pue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367EC23B-D432-4AC3-9C68-9F10790532BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3FEB5F-B108-4897-8AAE-7BD15C7BAF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,11 @@
   </sheets>
   <definedNames>
     <definedName name="PUE.NUM.edad2">Sheet1!$D$4</definedName>
+    <definedName name="PUE.NUM.legajos">Sheet1!$A$3:$A$5</definedName>
     <definedName name="PUE.SLIDE.0.1.0.1.porcentaje1">Sheet1!$B$11</definedName>
     <definedName name="PUE.STRING.cadena1">Sheet1!$G$11</definedName>
     <definedName name="PUE.SWITCH.analizar">Sheet1!$E$14</definedName>
+    <definedName name="PUE.SWITCH.booleanos">Sheet1!$I$9:$I$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nombre</t>
   </si>
@@ -89,6 +91,27 @@
   </si>
   <si>
     <t>Hola</t>
+  </si>
+  <si>
+    <t>LEGAJOS</t>
+  </si>
+  <si>
+    <t>Maquina 1</t>
+  </si>
+  <si>
+    <t>Maquina 2</t>
+  </si>
+  <si>
+    <t>Maquina 3</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Anios</t>
   </si>
 </sst>
 </file>
@@ -160,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +198,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O14"/>
+  <dimension ref="A2:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +496,10 @@
     <col min="14" max="14" width="11.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -484,15 +514,24 @@
       </c>
       <c r="F2" s="6"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>25407</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -507,15 +546,26 @@
       </c>
       <c r="F3" s="6"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="I3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="9">
+        <v>100</v>
+      </c>
+      <c r="K3" s="9">
+        <v>200</v>
+      </c>
+      <c r="L3" s="9">
+        <v>700</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>26549</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -530,15 +580,26 @@
       </c>
       <c r="F4" s="6"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="I4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.5</v>
+      </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>23403</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
@@ -553,15 +614,23 @@
       </c>
       <c r="F5" s="6"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="I5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9">
+        <v>2</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
@@ -578,40 +647,52 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>0.3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I11" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I12" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="b">
-        <v>1</v>
+      <c r="E14" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -622,6 +703,6 @@
     <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>